<commit_message>
Assigned stories and tasks for sprint 4
</commit_message>
<xml_diff>
--- a/Scrum/Milestone 3/Sprint 4 Backlog.xlsx
+++ b/Scrum/Milestone 3/Sprint 4 Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\Desktop\SEPT\Scrum\Milestone 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD24912-63AD-4D8F-97E0-FF63A1991717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE53E84-EF3E-4C49-960B-CA50DEEF3EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17640" yWindow="2430" windowWidth="12840" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="47">
   <si>
     <t>PBI ID</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>SPRINT #4 BACKLOG</t>
+  </si>
+  <si>
+    <t>Jared</t>
+  </si>
+  <si>
+    <t>Shannon</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Aili</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1479,7 @@
   <dimension ref="B1:J40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1544,7 +1556,9 @@
       <c r="E5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="G5" s="25"/>
       <c r="H5" s="20" t="s">
         <v>9</v>
@@ -1561,7 +1575,9 @@
       <c r="E6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="G6" s="25"/>
       <c r="H6" s="20" t="s">
         <v>9</v>
@@ -1578,7 +1594,9 @@
       <c r="E7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="G7" s="25"/>
       <c r="H7" s="20" t="s">
         <v>9</v>
@@ -1599,7 +1617,9 @@
       <c r="E8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G8" s="21"/>
       <c r="H8" s="20" t="s">
         <v>9</v>
@@ -1616,7 +1636,9 @@
       <c r="E9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G9" s="21"/>
       <c r="H9" s="20" t="s">
         <v>9</v>
@@ -1633,7 +1655,9 @@
       <c r="E10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G10" s="21"/>
       <c r="H10" s="20" t="s">
         <v>9</v>
@@ -1654,7 +1678,9 @@
       <c r="E11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G11" s="21"/>
       <c r="H11" s="20" t="s">
         <v>9</v>
@@ -1671,7 +1697,9 @@
       <c r="E12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G12" s="21"/>
       <c r="H12" s="20" t="s">
         <v>9</v>
@@ -1688,7 +1716,9 @@
       <c r="E13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G13" s="21"/>
       <c r="H13" s="20" t="s">
         <v>9</v>
@@ -1709,7 +1739,9 @@
       <c r="E14" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G14" s="21"/>
       <c r="H14" s="20" t="s">
         <v>9</v>
@@ -1726,7 +1758,9 @@
       <c r="E15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="21"/>
       <c r="H15" s="20" t="s">
         <v>9</v>
@@ -1743,7 +1777,9 @@
       <c r="E16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="21"/>
       <c r="H16" s="20" t="s">
         <v>9</v>
@@ -1764,7 +1800,9 @@
       <c r="E17" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G17" s="21"/>
       <c r="H17" s="20" t="s">
         <v>9</v>
@@ -1781,7 +1819,9 @@
       <c r="E18" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G18" s="21"/>
       <c r="H18" s="20" t="s">
         <v>9</v>
@@ -1798,7 +1838,9 @@
       <c r="E19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="G19" s="21"/>
       <c r="H19" s="20" t="s">
         <v>9</v>
@@ -1819,7 +1861,9 @@
       <c r="E20" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="G20" s="21"/>
       <c r="H20" s="20" t="s">
         <v>9</v>
@@ -1836,7 +1880,9 @@
       <c r="E21" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="G21" s="21"/>
       <c r="H21" s="20" t="s">
         <v>9</v>
@@ -1853,7 +1899,9 @@
       <c r="E22" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20" t="s">
         <v>9</v>
@@ -1874,7 +1922,9 @@
       <c r="E23" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="21"/>
       <c r="H23" s="20" t="s">
         <v>9</v>
@@ -1891,7 +1941,9 @@
       <c r="E24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G24" s="21"/>
       <c r="H24" s="20" t="s">
         <v>9</v>
@@ -1908,7 +1960,9 @@
       <c r="E25" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G25" s="21"/>
       <c r="H25" s="20" t="s">
         <v>9</v>
@@ -1929,7 +1983,9 @@
       <c r="E26" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G26" s="21"/>
       <c r="H26" s="20" t="s">
         <v>9</v>
@@ -1946,7 +2002,9 @@
       <c r="E27" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G27" s="21"/>
       <c r="H27" s="20" t="s">
         <v>9</v>
@@ -1963,7 +2021,9 @@
       <c r="E28" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20" t="s">
         <v>9</v>
@@ -1984,7 +2044,9 @@
       <c r="E29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G29" s="21"/>
       <c r="H29" s="20" t="s">
         <v>9</v>
@@ -2001,7 +2063,9 @@
       <c r="E30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G30" s="21"/>
       <c r="H30" s="20" t="s">
         <v>9</v>
@@ -2018,7 +2082,9 @@
       <c r="E31" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="14"/>
+      <c r="F31" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G31" s="21"/>
       <c r="H31" s="20" t="s">
         <v>9</v>
@@ -2039,7 +2105,9 @@
       <c r="E32" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G32" s="21"/>
       <c r="H32" s="20" t="s">
         <v>9</v>
@@ -2056,7 +2124,9 @@
       <c r="E33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="14"/>
+      <c r="F33" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="20" t="s">
         <v>9</v>
@@ -2073,7 +2143,9 @@
       <c r="E34" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G34" s="14"/>
       <c r="H34" s="20" t="s">
         <v>9</v>
@@ -2094,7 +2166,9 @@
       <c r="E35" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G35" s="21"/>
       <c r="H35" s="20" t="s">
         <v>9</v>
@@ -2111,7 +2185,9 @@
       <c r="E36" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="14"/>
+      <c r="F36" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G36" s="21"/>
       <c r="H36" s="20" t="s">
         <v>9</v>
@@ -2128,7 +2204,9 @@
       <c r="E37" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="G37" s="21"/>
       <c r="H37" s="20" t="s">
         <v>9</v>
@@ -2149,7 +2227,9 @@
       <c r="E38" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G38" s="21"/>
       <c r="H38" s="20" t="s">
         <v>9</v>
@@ -2166,7 +2246,9 @@
       <c r="E39" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="14"/>
+      <c r="F39" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G39" s="21"/>
       <c r="H39" s="20" t="s">
         <v>9</v>
@@ -2183,7 +2265,9 @@
       <c r="E40" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="14"/>
+      <c r="F40" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="G40" s="21"/>
       <c r="H40" s="20" t="s">
         <v>9</v>
@@ -3471,21 +3555,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD6B7AE05836784DB9DDF79838E135B0" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56f2e1d40083bc882c879fd5f0e30a2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1977bc59-59cf-46de-bb10-abef6dc3255c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="917e586b705a352b9e3a8a8ba2891683" ns2:_="">
     <xsd:import namespace="1977bc59-59cf-46de-bb10-abef6dc3255c"/>
@@ -3657,24 +3726,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C82FB4F2-286A-40A1-8011-220F672FEF88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E11F8907-776F-44AD-B681-425AE9F3D166}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C28FE173-FBF3-44D6-AF77-81820CDE339A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3690,4 +3757,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E11F8907-776F-44AD-B681-425AE9F3D166}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C82FB4F2-286A-40A1-8011-220F672FEF88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>